<commit_message>
update: Transaksi Penjualan and fixing some code
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_pembayaran.xlsx
+++ b/PWL_POS/public/template_pembayaran.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_Necha\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A8514-4398-4FA2-9695-1EBC0AB3C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6291EC9-98C7-4DDA-9DEB-019ACA86EFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F338FED4-E3D7-41F7-98BC-CBD0ED3156CD}"/>
+    <workbookView xWindow="10905" yWindow="375" windowWidth="9585" windowHeight="11145" xr2:uid="{F338FED4-E3D7-41F7-98BC-CBD0ED3156CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="4">
-        <v>45760</v>
+        <v>45759</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -534,18 +534,18 @@
         <v>2</v>
       </c>
       <c r="F3" s="4">
-        <v>45761</v>
+        <v>45760</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3">
-        <v>70000</v>
+        <v>40000</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="4">
-        <v>45762</v>
+        <v>45760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>